<commit_message>
update the upload files
</commit_message>
<xml_diff>
--- a/data_uploads/nodes_pue_irri_inputs.xlsx
+++ b/data_uploads/nodes_pue_irri_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuezi/Library/CloudStorage/GoogleDrive-yw3054@columbia.edu/My Drive/LAB/Flexible_load_paper/model/rural_energy_planning_model/data_uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB39E9A5-C4D4-DD4B-B350-2D981FEC10AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BC9CDD-819B-054D-B700-B01F9C980E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30160" yWindow="14820" windowWidth="23180" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="11080" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes_inputs" sheetId="1" r:id="rId1"/>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="A1:G2"/>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -906,7 +906,7 @@
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>